<commit_message>
work on script to generate-glyph-excel-sheet. saving work
</commit_message>
<xml_diff>
--- a/generated/font-merging/glyph-groups.xlsx
+++ b/generated/font-merging/glyph-groups.xlsx
@@ -1,15 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Intro1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Intro" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Intro35" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Intro34" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Intro33" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Intro32" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Intro31" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Intro30" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Intro29" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Intro28" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Intro27" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Intro26" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Intro25" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Intro24" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Intro23" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Intro22" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Intro21" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Intro20" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Intro19" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Intro18" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Intro17" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Intro16" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Intro15" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="Intro14" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="Intro13" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="Intro12" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="Intro11" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="Intro10" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="Intro9" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="Intro8" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="Intro7" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="Intro6" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="Intro5" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="Intro4" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="Intro3" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="Intro2" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="Intro1" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="Intro" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="Sheet" sheetId="37" state="visible" r:id="rId37"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +461,511 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -458,14 +996,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Each glyph is represented by the md5 of the glyph components, the glyph image, and the names given to this glyph as duplicates are often present with different names.</t>
+          <t>Each glyph is represented by the glyph image, the md5 of the glyph components, the rasm group name, the ijam group name, the harakat group name, and the set of names given to this glyph.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Each distributor's glyphs initially begin in the unsorted column and then by hand are sorted into distinct groups based on characteristcs such as rasm.</t>
+          <t>Each distributor's glyphs initially begin in the unsorted column and then by hand are sorted into distinct groups based on characteristics</t>
         </is>
       </c>
     </row>
@@ -474,7 +1012,115 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>